<commit_message>
update @story description and snc-uibackend-relationCheck-Test-7 case
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-ui-backend-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-ui-backend-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FE4839-A4BF-4CB1-B553-9AD453DA3D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D44EADF-BA5D-44D9-93D6-38BC5B8E261A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-14570" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="graphsEntityCheck" sheetId="1" r:id="rId1"/>
@@ -931,12 +931,20 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Entity Battery(id:4195) ’s property has empty or illegal name, please modify.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity test(id:e-9166) ’s property has empty or illegal name, please modify.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>{
 "entities": [],
 	"relations": [{
 		"id": "edge-0.68325641574748961640140543242",
-		"in": "761",
-		"out": "760",
+		"in": "$entity_id2",
+		"out": "$entity_id1",
 		"properties": {
 			"keytype": "fk",
 			"relation": "one-to-one"
@@ -945,14 +953,6 @@
 		"removeStatus": false
 	}]
 }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity Battery(id:4195) ’s property has empty or illegal name, please modify.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity test(id:e-9166) ’s property has empty or illegal name, please modify.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1344,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1653,7 +1653,7 @@
         <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="207" x14ac:dyDescent="0.25">
@@ -1676,7 +1676,7 @@
         <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="234.6" x14ac:dyDescent="0.25">
@@ -1789,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF9EE4B-979F-4E8E-95DA-19E502E27CF7}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1970,7 +1970,7 @@
         <v>85</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D8">
         <v>200</v>

</xml_diff>

<commit_message>
update @story and $edge_id1 into correct value
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-ui-backend-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-ui-backend-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D44EADF-BA5D-44D9-93D6-38BC5B8E261A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866CFD0C-BBD3-4A47-A7C4-081B7E209525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-14570" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,10 +522,360 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>The name of relation (id:edge-333ad44c-f55e-48c2-a55c-20a17e5c60a6) is empty or illegal, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relation name empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-2</t>
+  </si>
+  <si>
+    <t>relation name illegal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The name of relation !@(id:edge-333ad44c-f55e-48c2-a55c-20a17e5c60a6) is empty or illegal, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-3</t>
+  </si>
+  <si>
+    <t>relation name chinese illegal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The name of relation 中文(id:edge-333ad44c-f55e-48c2-a55c-20a17e5c60a6) is empty or illegal, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-4</t>
+  </si>
+  <si>
+    <t>relation conflict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>{
 	"entities": [],
 	"relations": [{
-		"id": "$edeg_id1",
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "$entity_id2",
+		"out": "$entity_id1",
+		"properties": {
+			"keytype": "fk",
+			"relation": "one-to-one",
+			"typevalue": "type:type"
+		},
+		"label": "gp_edge1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The name of relation gp_edge1(id:edge-0.68325641574748961640140543242)  conflicts with other relations between same endpoints，please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-5</t>
+  </si>
+  <si>
+    <t>relation lack property field</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"entities": [],
+	"relations": [{
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "$entity_id2",
+		"out": "$entity_id1",
+		"properties": {
+			"keytype": "fk",
+			"typevalue": "type:type"
+		},
+		"label": "new1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Relation new1(id:edge-0.68325641574748961640140543242) lacks property fields [relation]，[keytype] or [typevalue], please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-6</t>
+  </si>
+  <si>
+    <t>{
+	"entities": [],
+	"relations": [{
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "$entity_id2",
+		"out": "$entity_id1",
+		"properties": {
+			"relation": "one-to-one",
+			"typevalue": "type:type"
+		},
+		"label": "new1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-7</t>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-8</t>
+  </si>
+  <si>
+    <t>relation properties empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"entities": [],
+	"relations": [{
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "$entity_id2",
+		"out": "$entity_id1",
+		"properties": {
+			"keytype": "fk",
+			"relation": "",
+			"typevalue": "type:type"
+		},
+		"label": "new1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Relation new1(id:edge-0.68325641574748961640140543242)  has no or incomplete association field, please modify</t>
+  </si>
+  <si>
+    <t>Relation new1(id:edge-0.68325641574748961640140543242)  has no or incomplete association field, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-9</t>
+  </si>
+  <si>
+    <t>relation properties value invalid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"entities": [],
+	"relations": [{
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "$entity_id2",
+		"out": "$entity_id1",
+		"properties": {
+			"keytype": "fk",
+			"relation": "many-to-many",
+			"typevalue": "type:type"
+		},
+		"label": "new1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-10</t>
+  </si>
+  <si>
+    <t>relation keytype value empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"entities": [],
+	"relations": [{
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "$entity_id2",
+		"out": "$entity_id1",
+		"properties": {
+			"keytype": "",
+			"relation": "one-to-many",
+			"typevalue": "type:type"
+		},
+		"label": "new1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The keytype of relation new1(id:edge-0.68325641574748961640140543242)  is empty or illegal, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-11</t>
+  </si>
+  <si>
+    <t>relation keytype value invalid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"entities": [],
+	"relations": [{
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "$entity_id2",
+		"out": "$entity_id1",
+		"properties": {
+			"keytype": "test",
+			"relation": "one-to-many",
+			"typevalue": "type:type"
+		},
+		"label": "new1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relation typevalue not exist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-12</t>
+  </si>
+  <si>
+    <t>{
+	"entities": [],
+	"relations": [{
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "$entity_id2",
+		"out": "$entity_id1",
+		"properties": {
+			"keytype": "fk",
+			"relation": "one-to-many",
+			"typevalue": "test1:test2"
+		},
+		"label": "new1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity new1(id:edge-0.68325641574748961640140543242) ’s association field does not exist, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-13</t>
+  </si>
+  <si>
+    <t>good request, no relation in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"entities": [],
+	"relations": [{
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "",
+		"out": "$entity_id1",
+		"properties": {
+			"keytype": "fk",
+			"relation": "one-to-one",
+			"typevalue": "type:type"
+		},
+		"label": "new1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-14</t>
+  </si>
+  <si>
+    <t>good request, no relation out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"entities": [],
+	"relations": [{
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "$entity_id1",
+		"out": "",
+		"properties": {
+			"keytype": "fk",
+			"relation": "one-to-one",
+			"typevalue": "type:type"
+		},
+		"label": "new1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snc-uibackend-relationCheck-Test-15</t>
+  </si>
+  <si>
+    <t>goood request, relation in not exist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"entities": [],
+	"relations": [{
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "999999",
+		"out": "$entity_id1",
+		"properties": {
+			"keytype": "fk",
+			"relation": "one-to-one",
+			"typevalue": "type:type"
+		},
+		"label": "new1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity Battery(id:4195) ’s property has empty or illegal name, please modify.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity test(id:e-9166) ’s property has empty or illegal name, please modify.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+"entities": [],
+	"relations": [{
+		"id": "edge-0.68325641574748961640140543242",
+		"in": "$entity_id2",
+		"out": "$entity_id1",
+		"properties": {
+			"keytype": "fk",
+			"relation": "one-to-one"
+		},
+		"label": "new1",
+		"removeStatus": false
+	}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"entities": [],
+	"relations": [{
+		"id": "$edge_id1",
 		"in": "$entity_id2",
 		"out": "$entity_id1",
 		"properties": {
@@ -547,28 +897,12 @@
 		"removeStatus": false
 	}]
 }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The name of relation (id:edge-333ad44c-f55e-48c2-a55c-20a17e5c60a6) is empty or illegal, please modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>relation name empty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-2</t>
-  </si>
-  <si>
-    <t>relation name illegal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>{
 	"entities": [],
 	"relations": [{
-		"id": "$edeg_id1",
+		"id": "$edge_id1",
 		"in": "$entity_id2",
 		"out": "$entity_id1",
 		"properties": {
@@ -590,24 +924,12 @@
 		"removeStatus": false
 	}]
 }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The name of relation !@(id:edge-333ad44c-f55e-48c2-a55c-20a17e5c60a6) is empty or illegal, please modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-3</t>
-  </si>
-  <si>
-    <t>relation name chinese illegal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>{
 	"entities": [],
 	"relations": [{
-		"id": "$edeg_id1",
+		"id": "$edge_id1",
 		"in": "$entity_id2",
 		"out": "$entity_id1",
 		"properties": {
@@ -629,331 +951,6 @@
 		"removeStatus": false
 	}]
 }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The name of relation 中文(id:edge-333ad44c-f55e-48c2-a55c-20a17e5c60a6) is empty or illegal, please modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-4</t>
-  </si>
-  <si>
-    <t>relation conflict</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-	"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "$entity_id2",
-		"out": "$entity_id1",
-		"properties": {
-			"keytype": "fk",
-			"relation": "one-to-one",
-			"typevalue": "type:type"
-		},
-		"label": "gp_edge1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The name of relation gp_edge1(id:edge-0.68325641574748961640140543242)  conflicts with other relations between same endpoints，please modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-5</t>
-  </si>
-  <si>
-    <t>relation lack property field</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-	"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "$entity_id2",
-		"out": "$entity_id1",
-		"properties": {
-			"keytype": "fk",
-			"typevalue": "type:type"
-		},
-		"label": "new1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Relation new1(id:edge-0.68325641574748961640140543242) lacks property fields [relation]，[keytype] or [typevalue], please modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-6</t>
-  </si>
-  <si>
-    <t>{
-	"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "$entity_id2",
-		"out": "$entity_id1",
-		"properties": {
-			"relation": "one-to-one",
-			"typevalue": "type:type"
-		},
-		"label": "new1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-7</t>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-8</t>
-  </si>
-  <si>
-    <t>relation properties empty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-	"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "$entity_id2",
-		"out": "$entity_id1",
-		"properties": {
-			"keytype": "fk",
-			"relation": "",
-			"typevalue": "type:type"
-		},
-		"label": "new1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Relation new1(id:edge-0.68325641574748961640140543242)  has no or incomplete association field, please modify</t>
-  </si>
-  <si>
-    <t>Relation new1(id:edge-0.68325641574748961640140543242)  has no or incomplete association field, please modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-9</t>
-  </si>
-  <si>
-    <t>relation properties value invalid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-	"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "$entity_id2",
-		"out": "$entity_id1",
-		"properties": {
-			"keytype": "fk",
-			"relation": "many-to-many",
-			"typevalue": "type:type"
-		},
-		"label": "new1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-10</t>
-  </si>
-  <si>
-    <t>relation keytype value empty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-	"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "$entity_id2",
-		"out": "$entity_id1",
-		"properties": {
-			"keytype": "",
-			"relation": "one-to-many",
-			"typevalue": "type:type"
-		},
-		"label": "new1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The keytype of relation new1(id:edge-0.68325641574748961640140543242)  is empty or illegal, please modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-11</t>
-  </si>
-  <si>
-    <t>relation keytype value invalid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-	"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "$entity_id2",
-		"out": "$entity_id1",
-		"properties": {
-			"keytype": "test",
-			"relation": "one-to-many",
-			"typevalue": "type:type"
-		},
-		"label": "new1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>relation typevalue not exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-12</t>
-  </si>
-  <si>
-    <t>{
-	"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "$entity_id2",
-		"out": "$entity_id1",
-		"properties": {
-			"keytype": "fk",
-			"relation": "one-to-many",
-			"typevalue": "test1:test2"
-		},
-		"label": "new1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity new1(id:edge-0.68325641574748961640140543242) ’s association field does not exist, please modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-13</t>
-  </si>
-  <si>
-    <t>good request, no relation in</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-	"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "",
-		"out": "$entity_id1",
-		"properties": {
-			"keytype": "fk",
-			"relation": "one-to-one",
-			"typevalue": "type:type"
-		},
-		"label": "new1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-14</t>
-  </si>
-  <si>
-    <t>good request, no relation out</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-	"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "$entity_id1",
-		"out": "",
-		"properties": {
-			"keytype": "fk",
-			"relation": "one-to-one",
-			"typevalue": "type:type"
-		},
-		"label": "new1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snc-uibackend-relationCheck-Test-15</t>
-  </si>
-  <si>
-    <t>goood request, relation in not exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-	"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "999999",
-		"out": "$entity_id1",
-		"properties": {
-			"keytype": "fk",
-			"relation": "one-to-one",
-			"typevalue": "type:type"
-		},
-		"label": "new1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity Battery(id:4195) ’s property has empty or illegal name, please modify.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity test(id:e-9166) ’s property has empty or illegal name, please modify.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-"entities": [],
-	"relations": [{
-		"id": "edge-0.68325641574748961640140543242",
-		"in": "$entity_id2",
-		"out": "$entity_id1",
-		"properties": {
-			"keytype": "fk",
-			"relation": "one-to-one"
-		},
-		"label": "new1",
-		"removeStatus": false
-	}]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1344,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1653,7 +1650,7 @@
         <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="207" x14ac:dyDescent="0.25">
@@ -1676,7 +1673,7 @@
         <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="234.6" x14ac:dyDescent="0.25">
@@ -1789,8 +1786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF9EE4B-979F-4E8E-95DA-19E502E27CF7}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1829,10 +1826,10 @@
         <v>68</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>6</v>
@@ -1844,18 +1841,18 @@
         <v>8</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="345" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
         <v>72</v>
       </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="D3">
         <v>200</v>
@@ -1867,18 +1864,18 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="345" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="D4">
         <v>200</v>
@@ -1890,18 +1887,18 @@
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D5">
         <v>200</v>
@@ -1913,18 +1910,18 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="193.2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D6">
         <v>200</v>
@@ -1936,18 +1933,18 @@
         <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D7">
         <v>200</v>
@@ -1959,18 +1956,18 @@
         <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="193.2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D8">
         <v>200</v>
@@ -1982,18 +1979,18 @@
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D9">
         <v>200</v>
@@ -2005,18 +2002,18 @@
         <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D10">
         <v>200</v>
@@ -2028,18 +2025,18 @@
         <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -2051,18 +2048,18 @@
         <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D12">
         <v>200</v>
@@ -2074,18 +2071,18 @@
         <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D13">
         <v>200</v>
@@ -2097,18 +2094,18 @@
         <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D14">
         <v>200</v>
@@ -2122,13 +2119,13 @@
     </row>
     <row r="15" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D15">
         <v>200</v>
@@ -2142,13 +2139,13 @@
     </row>
     <row r="16" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D16">
         <v>200</v>

</xml_diff>

<commit_message>
update for ui-workbench internal release
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-ui-backend-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-ui-backend-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866CFD0C-BBD3-4A47-A7C4-081B7E209525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AEF9D0-B3B1-4A9E-AEFB-1F31584126DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-14570" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-14560" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="graphsEntityCheck" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="124">
   <si>
     <t>test-id</t>
   </si>
@@ -277,10 +277,6 @@
     <t>snc-uibackend-graphsCheck-Test-8</t>
   </si>
   <si>
-    <t>has no or incomplete association field</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{
     "entities": [
         {
@@ -299,9 +295,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Entity test(id:e-9166)  has no or incomplete association field, please modify</t>
-  </si>
-  <si>
     <t>snc-uibackend-graphsCheck-Test-9</t>
   </si>
   <si>
@@ -320,10 +313,6 @@
     ],
     "relations": []
 }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Entity test(id:e-9166)  has no or incomplete association field, please modify</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -657,13 +646,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Relation new1(id:edge-0.68325641574748961640140543242)  has no or incomplete association field, please modify</t>
-  </si>
-  <si>
-    <t>Relation new1(id:edge-0.68325641574748961640140543242)  has no or incomplete association field, please modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>snc-uibackend-relationCheck-Test-9</t>
   </si>
   <si>
@@ -951,6 +933,34 @@
 		"removeStatus": false
 	}]
 }</t>
+  </si>
+  <si>
+    <t>The type of entity test(id:e-9166)  is empty or illegal, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is empty or illegal, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The type of entity test(id:e-9166)  is empty or illegal, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The primary key of entity test(id:e-9166)  is empty or illegal, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> is empty or illegal, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The relation type of relation new1(id:edge-0.68325641574748961640140543242)  is empty or illegal, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The relation type of relation new1(id:edge-0.68325641574748961640140543242)  is empty or illegal, please modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1341,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1543,10 +1553,10 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="D9">
         <v>200</v>
@@ -1558,18 +1568,18 @@
         <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="220.8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10">
         <v>200</v>
@@ -1581,18 +1591,18 @@
         <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>121</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -1604,18 +1614,18 @@
         <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="193.2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D12">
         <v>200</v>
@@ -1627,18 +1637,18 @@
         <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D13">
         <v>200</v>
@@ -1650,18 +1660,18 @@
         <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D14">
         <v>200</v>
@@ -1673,18 +1683,18 @@
         <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="234.6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D15">
         <v>200</v>
@@ -1696,7 +1706,7 @@
         <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1734,10 +1744,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1751,19 +1761,19 @@
     </row>
     <row r="2" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>6</v>
@@ -1786,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF9EE4B-979F-4E8E-95DA-19E502E27CF7}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1823,13 +1833,13 @@
     </row>
     <row r="2" spans="1:7" ht="330" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>6</v>
@@ -1841,18 +1851,18 @@
         <v>8</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="345" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D3">
         <v>200</v>
@@ -1864,18 +1874,18 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="345" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D4">
         <v>200</v>
@@ -1887,18 +1897,18 @@
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D5">
         <v>200</v>
@@ -1910,18 +1920,18 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="193.2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D6">
         <v>200</v>
@@ -1933,18 +1943,18 @@
         <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D7">
         <v>200</v>
@@ -1956,18 +1966,18 @@
         <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="193.2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D8">
         <v>200</v>
@@ -1979,18 +1989,18 @@
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D9">
         <v>200</v>
@@ -2002,18 +2012,18 @@
         <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D10">
         <v>200</v>
@@ -2025,18 +2035,18 @@
         <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -2048,18 +2058,18 @@
         <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D12">
         <v>200</v>
@@ -2071,18 +2081,18 @@
         <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D13">
         <v>200</v>
@@ -2094,18 +2104,18 @@
         <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D14">
         <v>200</v>
@@ -2119,13 +2129,13 @@
     </row>
     <row r="15" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D15">
         <v>200</v>
@@ -2139,13 +2149,13 @@
     </row>
     <row r="16" spans="1:7" ht="207" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D16">
         <v>200</v>

</xml_diff>